<commit_message>
Update example and answer question
</commit_message>
<xml_diff>
--- a/NOTE_OCA.xlsx
+++ b/NOTE_OCA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="399">
   <si>
     <t>1.1 Comments:</t>
   </si>
@@ -1112,14 +1112,122 @@
     <t>Một abstract class có thể khai báo abstract method hoặc ko khai báo</t>
   </si>
   <si>
-    <t>Class con extend abstract class không thể khai báo abstract method</t>
+    <t>Một concrete class (kế thừa hoặc implement abstract method) không thể khai báo abtract method</t>
+  </si>
+  <si>
+    <t>Abstract Interface</t>
+  </si>
+  <si>
+    <t>Một interface mặc định là abstract, kể cả có khai báo thêm từ khóa abstract hay không thì vẫn compile OK</t>
+  </si>
+  <si>
+    <t>Abstract method</t>
+  </si>
+  <si>
+    <t>Chỉ xuất hiện ở Abstract class</t>
+  </si>
+  <si>
+    <t>Không có body</t>
+  </si>
+  <si>
+    <t>2. Từ khóa final</t>
+  </si>
+  <si>
+    <t>Chỉ apply được với class, variable, method</t>
+  </si>
+  <si>
+    <t>Không apply được với interface</t>
+  </si>
+  <si>
+    <t>Final Class</t>
+  </si>
+  <si>
+    <t>Không thể được phép kế thừa class khác</t>
+  </si>
+  <si>
+    <t>final Method</t>
+  </si>
+  <si>
+    <t>Không thể bị ghi đè</t>
+  </si>
+  <si>
+    <t>Final variable</t>
+  </si>
+  <si>
+    <t>Không thể thay đổi giá trị (đối với biến local, class variable)</t>
+  </si>
+  <si>
+    <t>class Person {</t>
+  </si>
+  <si>
+    <t>final StringBuilder name = new StringBuilder("Sh");</t>
+  </si>
+  <si>
+    <t>Person() {</t>
+  </si>
+  <si>
+    <t>name.append("reya");</t>
+  </si>
+  <si>
+    <t>name = new StringBuilder();</t>
+  </si>
+  <si>
+    <t>//  OK vì có thể dùng hàm để thay đổi giá trị</t>
+  </si>
+  <si>
+    <t>// NOT OK vì không thể assign một final object sang một object khác</t>
+  </si>
+  <si>
+    <t>3. Từ khóa static</t>
+  </si>
+  <si>
+    <t>Apply được với variables, methods, class, interface</t>
+  </si>
+  <si>
+    <t>Static variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Static variable đi theo class, </t>
+  </si>
+  <si>
+    <t>Static method</t>
+  </si>
+  <si>
+    <t>Non-static variable, Non-static method có thể truy cập static variable, static method</t>
+  </si>
+  <si>
+    <t>Tuy nhiên, ngược lại thì static variable, static method không thể truy cập tới non-static variable, non-static method</t>
+  </si>
+  <si>
+    <t>static class, static interface : Không đề cập đến trong phần thi OCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chỉ cần nhớ rule là static class, static interface không thể khai báo là top-level class, top-level interface </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ví dụ : </t>
+  </si>
+  <si>
+    <t>static class Address {}</t>
+  </si>
+  <si>
+    <t>static interface MyInterface {}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sai: </t>
+  </si>
+  <si>
+    <t>static class Person {}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1173,6 +1281,29 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1195,7 +1326,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1204,10 +1335,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1570,10 +1705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q503"/>
+  <dimension ref="A1:Q545"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A353" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K365" sqref="K365"/>
+    <sheetView tabSelected="1" topLeftCell="A395" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L411" sqref="L411"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2849,44 +2984,44 @@
       </c>
     </row>
     <row r="347" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="D347" s="9" t="s">
+      <c r="D347" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="E347" s="9"/>
-      <c r="F347" s="9" t="s">
+      <c r="E347" s="8"/>
+      <c r="F347" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="G347" s="9"/>
-      <c r="H347" s="9"/>
-      <c r="I347" s="9"/>
-      <c r="J347" s="9"/>
-      <c r="K347" s="9"/>
-      <c r="L347" s="9"/>
-      <c r="M347" s="9"/>
-      <c r="N347" s="9"/>
-      <c r="O347" s="9"/>
-      <c r="P347" s="9"/>
-      <c r="Q347" s="9"/>
+      <c r="G347" s="8"/>
+      <c r="H347" s="8"/>
+      <c r="I347" s="8"/>
+      <c r="J347" s="8"/>
+      <c r="K347" s="8"/>
+      <c r="L347" s="8"/>
+      <c r="M347" s="8"/>
+      <c r="N347" s="8"/>
+      <c r="O347" s="8"/>
+      <c r="P347" s="8"/>
+      <c r="Q347" s="8"/>
     </row>
     <row r="348" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="D348" s="9" t="s">
+      <c r="D348" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="E348" s="9"/>
-      <c r="F348" s="9" t="s">
+      <c r="E348" s="8"/>
+      <c r="F348" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="G348" s="9"/>
-      <c r="H348" s="9"/>
-      <c r="I348" s="9"/>
-      <c r="J348" s="9"/>
-      <c r="K348" s="9"/>
-      <c r="L348" s="9"/>
-      <c r="M348" s="9"/>
-      <c r="N348" s="9"/>
-      <c r="O348" s="9"/>
-      <c r="P348" s="9"/>
-      <c r="Q348" s="9"/>
+      <c r="G348" s="8"/>
+      <c r="H348" s="8"/>
+      <c r="I348" s="8"/>
+      <c r="J348" s="8"/>
+      <c r="K348" s="8"/>
+      <c r="L348" s="8"/>
+      <c r="M348" s="8"/>
+      <c r="N348" s="8"/>
+      <c r="O348" s="8"/>
+      <c r="P348" s="8"/>
+      <c r="Q348" s="8"/>
     </row>
     <row r="350" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C350" s="3" t="s">
@@ -3005,922 +3140,739 @@
     </row>
     <row r="367" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A367" s="2"/>
+      <c r="D367" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="F367" s="3" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="368" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A368" s="2"/>
     </row>
-    <row r="369" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A369" s="2"/>
-    </row>
-    <row r="370" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D369" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="F369" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="370" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A370" s="2"/>
-    </row>
-    <row r="371" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F370" s="3" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="371" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A371" s="2"/>
     </row>
-    <row r="372" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A372" s="2"/>
-    </row>
-    <row r="373" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C372" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="373" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A373" s="2"/>
-    </row>
-    <row r="374" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A374" s="6" t="s">
+      <c r="D373" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="374" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A374" s="2"/>
+      <c r="D374" s="3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="375" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A375" s="2"/>
+    </row>
+    <row r="376" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A376" s="2"/>
+      <c r="D376" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="F376" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="377" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A377" s="2"/>
+    </row>
+    <row r="378" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A378" s="2"/>
+      <c r="D378" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="F378" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="379" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A379" s="2"/>
+    </row>
+    <row r="380" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A380" s="2"/>
+      <c r="D380" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="F380" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="381" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A381" s="2"/>
+    </row>
+    <row r="382" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A382" s="2"/>
+      <c r="F382" s="3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A383" s="2"/>
+      <c r="G383" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A384" s="2"/>
+      <c r="G384" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="385" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A385" s="2"/>
+      <c r="H385" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="L385" s="9" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="386" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A386" s="2"/>
+      <c r="H386" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="L386" s="7" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="387" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A387" s="2"/>
+      <c r="G387" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="388" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A388" s="2"/>
+      <c r="F388" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="389" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A389" s="2"/>
+    </row>
+    <row r="390" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A390" s="2"/>
+      <c r="C390" s="3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="391" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A391" s="2"/>
+      <c r="D391" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="392" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A392" s="2"/>
+    </row>
+    <row r="393" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A393" s="2"/>
+      <c r="D393" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="F393" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="394" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A394" s="2"/>
+    </row>
+    <row r="395" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A395" s="2"/>
+      <c r="D395" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="396" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A396" s="2"/>
+    </row>
+    <row r="397" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A397" s="2"/>
+      <c r="E397" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="398" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A398" s="2"/>
+    </row>
+    <row r="399" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A399" s="2"/>
+      <c r="E399" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="400" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A400" s="2"/>
+    </row>
+    <row r="401" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A401" s="2"/>
+      <c r="D401" s="3" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="402" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A402" s="2"/>
+      <c r="E402" s="3" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="403" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A403" s="2"/>
+    </row>
+    <row r="404" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A404" s="2"/>
+    </row>
+    <row r="405" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A405" s="2"/>
+      <c r="E405" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="F405" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G405" s="12" t="s">
+        <v>377</v>
+      </c>
+      <c r="H405" s="13"/>
+      <c r="I405" s="13"/>
+      <c r="J405" s="13"/>
+    </row>
+    <row r="406" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A406" s="2"/>
+      <c r="G406" s="13"/>
+      <c r="H406" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="I406" s="13"/>
+      <c r="J406" s="13"/>
+    </row>
+    <row r="407" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A407" s="2"/>
+      <c r="G407" s="13"/>
+      <c r="H407" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="I407" s="13"/>
+      <c r="J407" s="13"/>
+    </row>
+    <row r="408" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A408" s="2"/>
+      <c r="G408" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="H408" s="13"/>
+      <c r="I408" s="13"/>
+      <c r="J408" s="13"/>
+    </row>
+    <row r="409" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A409" s="2"/>
+      <c r="G409" s="13"/>
+      <c r="H409" s="13"/>
+      <c r="I409" s="13"/>
+      <c r="J409" s="13"/>
+    </row>
+    <row r="410" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A410" s="2"/>
+      <c r="F410" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="G410" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="H410" s="13"/>
+      <c r="I410" s="13"/>
+      <c r="J410" s="13"/>
+    </row>
+    <row r="411" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A411" s="2"/>
+      <c r="G411" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="H411" s="13"/>
+      <c r="I411" s="13"/>
+      <c r="J411" s="13"/>
+    </row>
+    <row r="412" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A412" s="2"/>
+      <c r="G412" s="11"/>
+    </row>
+    <row r="413" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A413" s="2"/>
+      <c r="G413" s="11"/>
+    </row>
+    <row r="414" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A414" s="2"/>
+      <c r="G414" s="11"/>
+    </row>
+    <row r="415" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A415" s="2"/>
+      <c r="G415" s="11"/>
+    </row>
+    <row r="416" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A416" s="6" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="375" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B375" s="3">
+    <row r="417" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B417" s="3">
         <v>1</v>
       </c>
-      <c r="C375" s="3" t="s">
+      <c r="C417" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="D375" s="3" t="s">
+      <c r="D417" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="L375" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="376" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B376" s="3">
+      <c r="L417" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="418" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B418" s="3">
         <v>2</v>
-      </c>
-      <c r="C376" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="L376" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="377" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B377" s="3">
-        <v>3</v>
-      </c>
-      <c r="C377" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="L377" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="378" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B378" s="3">
-        <v>4</v>
-      </c>
-      <c r="C378" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="L378" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="379" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B379" s="3">
-        <v>5</v>
-      </c>
-      <c r="C379" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="L379" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="380" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B380" s="3">
-        <v>6</v>
-      </c>
-      <c r="C380" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="D380" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="E380" s="8"/>
-      <c r="F380" s="8"/>
-      <c r="G380" s="8"/>
-      <c r="H380" s="8"/>
-      <c r="I380" s="8"/>
-      <c r="J380" s="8"/>
-      <c r="K380" s="8"/>
-      <c r="L380" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="381" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B381" s="3">
-        <v>7</v>
-      </c>
-      <c r="C381" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="L381" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="382" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B382" s="3">
-        <v>8</v>
-      </c>
-      <c r="C382" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="L382" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="383" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B383" s="3">
-        <v>9</v>
-      </c>
-      <c r="C383" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="L383" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="384" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B384" s="3">
-        <v>10</v>
-      </c>
-      <c r="C384" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="L384" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="385" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B385" s="3">
-        <v>11</v>
-      </c>
-      <c r="C385" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="L385" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="386" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B386" s="3">
-        <v>12</v>
-      </c>
-      <c r="C386" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="D386" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="E386" s="8"/>
-      <c r="F386" s="8"/>
-      <c r="G386" s="8"/>
-      <c r="H386" s="8"/>
-      <c r="I386" s="8"/>
-      <c r="J386" s="8"/>
-      <c r="K386" s="8"/>
-      <c r="L386" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="387" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B387" s="3">
-        <v>13</v>
-      </c>
-      <c r="C387" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="L387" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="388" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B388" s="3">
-        <v>14</v>
-      </c>
-      <c r="C388" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="L388" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="389" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B389" s="3">
-        <v>15</v>
-      </c>
-      <c r="C389" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="D389" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="L389" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="390" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B390" s="3">
-        <v>16</v>
-      </c>
-      <c r="C390" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="L390" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="391" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B391" s="3">
-        <v>17</v>
-      </c>
-      <c r="C391" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="L391" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="392" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B392" s="3">
-        <v>18</v>
-      </c>
-      <c r="C392" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="D392" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="L392" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="393" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B393" s="3">
-        <v>19</v>
-      </c>
-      <c r="C393" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="D393" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="L393" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="394" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B394" s="3">
-        <v>20</v>
-      </c>
-      <c r="C394" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="D394" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="L394" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="395" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B395" s="3">
-        <v>21</v>
-      </c>
-      <c r="C395" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="L395" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="396" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B396" s="3">
-        <v>22</v>
-      </c>
-      <c r="C396" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="L396" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="397" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B397" s="3">
-        <v>23</v>
-      </c>
-      <c r="C397" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="D397" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="L397" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="398" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D398" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="400" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A400" s="6" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="401" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B401" s="3">
-        <v>1</v>
-      </c>
-      <c r="C401" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="D401" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="402" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B402" s="3">
-        <v>2</v>
-      </c>
-      <c r="C402" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="D402" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="403" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B403" s="3">
-        <v>3</v>
-      </c>
-      <c r="C403" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D403" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="404" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B404" s="3">
-        <v>4</v>
-      </c>
-      <c r="C404" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D404" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="405" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B405" s="3">
-        <v>5</v>
-      </c>
-      <c r="C405" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="D405" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="406" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B406" s="3">
-        <v>6</v>
-      </c>
-      <c r="C406" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D406" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="407" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B407" s="3">
-        <v>7</v>
-      </c>
-      <c r="C407" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="D407" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E407" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="408" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B408" s="3">
-        <v>8</v>
-      </c>
-      <c r="C408" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D408" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="409" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B409" s="3">
-        <v>9</v>
-      </c>
-      <c r="C409" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="D409" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="E409" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="410" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B410" s="3">
-        <v>10</v>
-      </c>
-      <c r="C410" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="D410" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E410" s="3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="411" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B411" s="3">
-        <v>11</v>
-      </c>
-      <c r="C411" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D411" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="412" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B412" s="3">
-        <v>12</v>
-      </c>
-      <c r="C412" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="D412" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="413" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B413" s="3">
-        <v>13</v>
-      </c>
-      <c r="C413" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="D413" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E413" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="414" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B414" s="3">
-        <v>14</v>
-      </c>
-      <c r="C414" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D414" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="415" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B415" s="3">
-        <v>15</v>
-      </c>
-      <c r="C415" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D415" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="416" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B416" s="3">
-        <v>16</v>
-      </c>
-      <c r="C416" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D416" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="417" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B417" s="3">
-        <v>17</v>
-      </c>
-      <c r="C417" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D417" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="418" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B418" s="3">
-        <v>18</v>
       </c>
       <c r="C418" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="D418" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="419" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="L418" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="419" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B419" s="3">
+        <v>3</v>
+      </c>
+      <c r="C419" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="L419" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="420" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B420" s="3">
+        <v>4</v>
+      </c>
+      <c r="C420" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="L420" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="421" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B421" s="3">
+        <v>5</v>
+      </c>
+      <c r="C421" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="L421" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="422" spans="2:12" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B422" s="3">
+        <v>6</v>
+      </c>
+      <c r="C422" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D422" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="E422" s="10"/>
+      <c r="F422" s="10"/>
+      <c r="G422" s="10"/>
+      <c r="H422" s="10"/>
+      <c r="I422" s="10"/>
+      <c r="J422" s="10"/>
+      <c r="K422" s="10"/>
+      <c r="L422" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="423" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B423" s="3">
+        <v>7</v>
+      </c>
+      <c r="C423" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="L423" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="424" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B424" s="3">
+        <v>8</v>
+      </c>
+      <c r="C424" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="L424" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="425" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B425" s="3">
+        <v>9</v>
+      </c>
+      <c r="C425" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="L425" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="426" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B426" s="3">
+        <v>10</v>
+      </c>
+      <c r="C426" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="L426" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="427" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B427" s="3">
+        <v>11</v>
+      </c>
+      <c r="C427" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="L427" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="428" spans="2:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B428" s="3">
+        <v>12</v>
+      </c>
+      <c r="C428" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D428" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="E428" s="10"/>
+      <c r="F428" s="10"/>
+      <c r="G428" s="10"/>
+      <c r="H428" s="10"/>
+      <c r="I428" s="10"/>
+      <c r="J428" s="10"/>
+      <c r="K428" s="10"/>
+      <c r="L428" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="429" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B429" s="3">
+        <v>13</v>
+      </c>
+      <c r="C429" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="L429" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="430" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B430" s="3">
+        <v>14</v>
+      </c>
+      <c r="C430" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="L430" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="431" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B431" s="3">
+        <v>15</v>
+      </c>
+      <c r="C431" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D431" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="L431" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="432" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B432" s="3">
+        <v>16</v>
+      </c>
+      <c r="C432" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="L432" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="433" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B433" s="3">
+        <v>17</v>
+      </c>
+      <c r="C433" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="L433" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="434" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B434" s="3">
+        <v>18</v>
+      </c>
+      <c r="C434" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D434" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="L434" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="435" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B435" s="3">
         <v>19</v>
       </c>
-      <c r="C419" s="3" t="s">
+      <c r="C435" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D435" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="L435" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="436" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B436" s="3">
+        <v>20</v>
+      </c>
+      <c r="C436" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D436" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="L436" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="437" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B437" s="3">
+        <v>21</v>
+      </c>
+      <c r="C437" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="D419" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="420" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B420" s="3">
-        <v>20</v>
-      </c>
-      <c r="C420" s="3" t="s">
+      <c r="L437" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="438" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B438" s="3">
+        <v>22</v>
+      </c>
+      <c r="C438" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="L438" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="439" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B439" s="3">
+        <v>23</v>
+      </c>
+      <c r="C439" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D439" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="L439" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="440" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D440" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="442" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A442" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="443" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B443" s="3">
+        <v>1</v>
+      </c>
+      <c r="C443" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D443" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="444" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B444" s="3">
+        <v>2</v>
+      </c>
+      <c r="C444" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D444" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="445" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B445" s="3">
+        <v>3</v>
+      </c>
+      <c r="C445" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D445" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="446" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B446" s="3">
+        <v>4</v>
+      </c>
+      <c r="C446" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="D420" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="421" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B421" s="3">
-        <v>21</v>
-      </c>
-      <c r="C421" s="3" t="s">
+      <c r="D446" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="447" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B447" s="3">
+        <v>5</v>
+      </c>
+      <c r="C447" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="D421" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="422" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B422" s="3">
-        <v>22</v>
-      </c>
-      <c r="C422" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="D422" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="423" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B423" s="3">
-        <v>23</v>
-      </c>
-      <c r="C423" s="3" t="s">
+      <c r="D447" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="448" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B448" s="3">
+        <v>6</v>
+      </c>
+      <c r="C448" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="D423" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="424" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B424" s="3">
-        <v>24</v>
-      </c>
-      <c r="C424" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="D424" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E424" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="425" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B425" s="3">
-        <v>25</v>
-      </c>
-      <c r="C425" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="D425" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="426" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B426" s="3">
-        <v>26</v>
-      </c>
-      <c r="C426" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="D426" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E426" s="3" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="427" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B427" s="3">
-        <v>27</v>
-      </c>
-      <c r="C427" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D427" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="428" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B428" s="3">
-        <v>28</v>
-      </c>
-      <c r="C428" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="D428" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E428" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="429" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B429" s="3">
-        <v>29</v>
-      </c>
-      <c r="C429" s="3" t="s">
+      <c r="D448" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="449" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B449" s="3">
+        <v>7</v>
+      </c>
+      <c r="C449" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D449" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E449" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="450" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B450" s="3">
+        <v>8</v>
+      </c>
+      <c r="C450" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="D429" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="430" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B430" s="3">
-        <v>30</v>
-      </c>
-      <c r="C430" s="3" t="s">
+      <c r="D450" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="451" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B451" s="3">
+        <v>9</v>
+      </c>
+      <c r="C451" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D451" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E451" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="452" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B452" s="3">
+        <v>10</v>
+      </c>
+      <c r="C452" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D452" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E452" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="453" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B453" s="3">
+        <v>11</v>
+      </c>
+      <c r="C453" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D430" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="431" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B431" s="3">
-        <v>31</v>
-      </c>
-      <c r="C431" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D431" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="432" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B432" s="3">
-        <v>32</v>
-      </c>
-      <c r="C432" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D432" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="433" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B433" s="3">
-        <v>33</v>
-      </c>
-      <c r="C433" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="D433" s="3" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="434" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B434" s="3">
-        <v>34</v>
-      </c>
-      <c r="C434" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D434" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="435" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B435" s="3">
-        <v>35</v>
-      </c>
-      <c r="C435" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="D435" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="436" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B436" s="3">
-        <v>36</v>
-      </c>
-      <c r="C436" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="D436" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="437" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B437" s="3">
-        <v>37</v>
-      </c>
-      <c r="C437" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="D437" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="438" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B438" s="3">
-        <v>38</v>
-      </c>
-      <c r="C438" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="D438" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="439" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B439" s="3">
-        <v>39</v>
-      </c>
-      <c r="C439" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D439" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="440" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B440" s="3">
-        <v>40</v>
-      </c>
-      <c r="C440" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="D440" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E440" s="3" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="441" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B441" s="3">
-        <v>41</v>
-      </c>
-      <c r="C441" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="D441" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="442" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B442" s="3">
-        <v>42</v>
-      </c>
-      <c r="C442" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="D442" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="443" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B443" s="3">
-        <v>43</v>
-      </c>
-      <c r="C443" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="D443" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="444" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B444" s="3">
-        <v>44</v>
-      </c>
-      <c r="C444" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D444" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="445" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B445" s="3">
-        <v>45</v>
-      </c>
-      <c r="C445" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="D445" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E445" s="3" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="446" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B446" s="3">
-        <v>46</v>
-      </c>
-      <c r="C446" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="D446" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="447" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B447" s="3">
-        <v>47</v>
-      </c>
-      <c r="C447" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D447" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="448" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B448" s="3">
-        <v>48</v>
-      </c>
-      <c r="C448" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="D448" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E448" s="3" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="449" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B449" s="3">
-        <v>49</v>
-      </c>
-      <c r="C449" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D449" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B450" s="3">
-        <v>50</v>
-      </c>
-      <c r="C450" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="D450" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E450" s="3" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A453" s="6" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="454" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D453" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="454" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B454" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C454" s="3" t="s">
         <v>222</v>
@@ -3929,184 +3881,175 @@
         <v>49</v>
       </c>
     </row>
-    <row r="455" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="455" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B455" s="3">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C455" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D455" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E455" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="456" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B456" s="3">
+        <v>14</v>
+      </c>
+      <c r="C456" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="D455" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="456" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B456" s="3">
-        <v>3</v>
-      </c>
-      <c r="C456" s="3" t="s">
+      <c r="D456" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="457" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B457" s="3">
+        <v>15</v>
+      </c>
+      <c r="C457" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D457" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="458" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B458" s="3">
+        <v>16</v>
+      </c>
+      <c r="C458" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D456" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="457" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B457" s="3">
-        <v>4</v>
-      </c>
-      <c r="C457" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D457" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="458" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B458" s="3">
-        <v>5</v>
-      </c>
-      <c r="C458" s="3" t="s">
-        <v>299</v>
-      </c>
       <c r="D458" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E458" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="459" spans="1:5" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="459" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B459" s="3">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C459" s="3" t="s">
-        <v>276</v>
+        <v>213</v>
       </c>
       <c r="D459" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E459" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="460" spans="1:5" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="460" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B460" s="3">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C460" s="3" t="s">
-        <v>258</v>
+        <v>213</v>
       </c>
       <c r="D460" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="461" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="461" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B461" s="3">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C461" s="3" t="s">
-        <v>302</v>
+        <v>222</v>
       </c>
       <c r="D461" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E461" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="462" spans="1:5" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="462" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B462" s="3">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C462" s="3" t="s">
-        <v>258</v>
+        <v>213</v>
       </c>
       <c r="D462" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="463" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="463" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B463" s="3">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C463" s="3" t="s">
-        <v>258</v>
+        <v>222</v>
       </c>
       <c r="D463" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="464" spans="1:5" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="464" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B464" s="3">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C464" s="3" t="s">
-        <v>213</v>
+        <v>269</v>
       </c>
       <c r="D464" s="3" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
     </row>
     <row r="465" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B465" s="3">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C465" s="3" t="s">
-        <v>304</v>
+        <v>213</v>
       </c>
       <c r="D465" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E465" s="3" t="s">
-        <v>305</v>
+        <v>49</v>
       </c>
     </row>
     <row r="466" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B466" s="3">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C466" s="3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="D466" s="3" t="s">
         <v>98</v>
       </c>
       <c r="E466" s="3" t="s">
-        <v>306</v>
+        <v>271</v>
       </c>
     </row>
     <row r="467" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B467" s="3">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C467" s="3" t="s">
-        <v>216</v>
+        <v>272</v>
       </c>
       <c r="D467" s="3" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
     </row>
     <row r="468" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B468" s="3">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C468" s="3" t="s">
-        <v>302</v>
+        <v>276</v>
       </c>
       <c r="D468" s="3" t="s">
-        <v>308</v>
+        <v>98</v>
       </c>
       <c r="E468" s="3" t="s">
-        <v>309</v>
+        <v>277</v>
       </c>
     </row>
     <row r="469" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B469" s="3">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C469" s="3" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D469" s="3" t="s">
         <v>49</v>
@@ -4114,21 +4057,24 @@
     </row>
     <row r="470" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B470" s="3">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C470" s="3" t="s">
-        <v>310</v>
+        <v>278</v>
       </c>
       <c r="D470" s="3" t="s">
         <v>98</v>
+      </c>
+      <c r="E470" s="3" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="471" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B471" s="3">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C471" s="3" t="s">
-        <v>213</v>
+        <v>258</v>
       </c>
       <c r="D471" s="3" t="s">
         <v>49</v>
@@ -4136,21 +4082,21 @@
     </row>
     <row r="472" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B472" s="3">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C472" s="3" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="D472" s="3" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
     </row>
     <row r="473" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B473" s="3">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C473" s="3" t="s">
-        <v>258</v>
+        <v>216</v>
       </c>
       <c r="D473" s="3" t="s">
         <v>49</v>
@@ -4158,10 +4104,10 @@
     </row>
     <row r="474" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B474" s="3">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C474" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D474" s="3" t="s">
         <v>49</v>
@@ -4169,21 +4115,21 @@
     </row>
     <row r="475" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B475" s="3">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C475" s="3" t="s">
-        <v>233</v>
+        <v>270</v>
       </c>
       <c r="D475" s="3" t="s">
-        <v>98</v>
+        <v>264</v>
       </c>
     </row>
     <row r="476" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B476" s="3">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C476" s="3" t="s">
-        <v>258</v>
+        <v>213</v>
       </c>
       <c r="D476" s="3" t="s">
         <v>49</v>
@@ -4191,10 +4137,10 @@
     </row>
     <row r="477" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B477" s="3">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C477" s="3" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="D477" s="3" t="s">
         <v>49</v>
@@ -4202,153 +4148,159 @@
     </row>
     <row r="478" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B478" s="3">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C478" s="3" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D478" s="3" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
     </row>
     <row r="479" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B479" s="3">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C479" s="3" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
       <c r="D479" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E479" s="3" t="s">
-        <v>313</v>
+        <v>49</v>
       </c>
     </row>
     <row r="480" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B480" s="3">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C480" s="3" t="s">
-        <v>280</v>
+        <v>222</v>
       </c>
       <c r="D480" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="481" spans="2:5" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="481" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B481" s="3">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C481" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D481" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="482" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B482" s="3">
+        <v>40</v>
+      </c>
+      <c r="C482" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D482" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E482" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="483" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B483" s="3">
+        <v>41</v>
+      </c>
+      <c r="C483" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D483" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="484" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B484" s="3">
+        <v>42</v>
+      </c>
+      <c r="C484" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D484" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="485" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B485" s="3">
+        <v>43</v>
+      </c>
+      <c r="C485" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="D485" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="486" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B486" s="3">
+        <v>44</v>
+      </c>
+      <c r="C486" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="D481" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="482" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B482" s="3">
-        <v>29</v>
-      </c>
-      <c r="C482" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D482" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="483" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B483" s="3">
-        <v>30</v>
-      </c>
-      <c r="C483" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="D483" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="484" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B484" s="3">
-        <v>31</v>
-      </c>
-      <c r="C484" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="D484" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="485" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B485" s="3">
-        <v>32</v>
-      </c>
-      <c r="C485" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="D485" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="486" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B486" s="3">
-        <v>33</v>
-      </c>
-      <c r="C486" s="3" t="s">
-        <v>222</v>
-      </c>
       <c r="D486" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="487" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B487" s="3">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C487" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D487" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E487" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="488" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B488" s="3">
+        <v>46</v>
+      </c>
+      <c r="C488" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D488" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="489" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B489" s="3">
+        <v>47</v>
+      </c>
+      <c r="C489" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D489" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="490" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B490" s="3">
+        <v>48</v>
+      </c>
+      <c r="C490" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="D487" s="3" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="488" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B488" s="3">
-        <v>35</v>
-      </c>
-      <c r="C488" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="D488" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="489" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B489" s="3">
-        <v>36</v>
-      </c>
-      <c r="C489" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D489" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="490" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B490" s="3">
-        <v>37</v>
-      </c>
-      <c r="C490" s="3" t="s">
-        <v>216</v>
-      </c>
       <c r="D490" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="491" spans="2:5" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="E490" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="491" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B491" s="3">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C491" s="3" t="s">
         <v>258</v>
@@ -4357,59 +4309,31 @@
         <v>49</v>
       </c>
     </row>
-    <row r="492" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B492" s="3">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C492" s="3" t="s">
-        <v>233</v>
+        <v>293</v>
       </c>
       <c r="D492" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="493" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B493" s="3">
-        <v>40</v>
-      </c>
-      <c r="C493" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D493" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="494" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B494" s="3">
-        <v>41</v>
-      </c>
-      <c r="C494" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="D494" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E494" s="3" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="495" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B495" s="3">
-        <v>42</v>
-      </c>
-      <c r="C495" s="3" t="s">
+      <c r="E492" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="495" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A495" s="6" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="496" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B496" s="3">
+        <v>1</v>
+      </c>
+      <c r="C496" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="D495" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="496" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B496" s="3">
-        <v>43</v>
-      </c>
-      <c r="C496" s="3" t="s">
-        <v>216</v>
       </c>
       <c r="D496" s="3" t="s">
         <v>49</v>
@@ -4417,74 +4341,71 @@
     </row>
     <row r="497" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B497" s="3">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="C497" s="3" t="s">
-        <v>270</v>
+        <v>213</v>
       </c>
       <c r="D497" s="3" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
     </row>
     <row r="498" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B498" s="3">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="C498" s="3" t="s">
-        <v>266</v>
+        <v>216</v>
       </c>
       <c r="D498" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E498" s="3" t="s">
-        <v>317</v>
+        <v>49</v>
       </c>
     </row>
     <row r="499" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B499" s="7">
-        <v>46</v>
-      </c>
-      <c r="C499" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="D499" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E499" s="7" t="s">
-        <v>318</v>
+      <c r="B499" s="3">
+        <v>4</v>
+      </c>
+      <c r="C499" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D499" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="500" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B500" s="3">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="C500" s="3" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="D500" s="3" t="s">
-        <v>49</v>
+        <v>98</v>
+      </c>
+      <c r="E500" s="3" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="501" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B501" s="3">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="C501" s="3" t="s">
-        <v>319</v>
+        <v>276</v>
       </c>
       <c r="D501" s="3" t="s">
         <v>98</v>
       </c>
       <c r="E501" s="3" t="s">
-        <v>320</v>
+        <v>301</v>
       </c>
     </row>
     <row r="502" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B502" s="3">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C502" s="3" t="s">
-        <v>216</v>
+        <v>258</v>
       </c>
       <c r="D502" s="3" t="s">
         <v>49</v>
@@ -4492,22 +4413,511 @@
     </row>
     <row r="503" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B503" s="3">
+        <v>8</v>
+      </c>
+      <c r="C503" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D503" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E503" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="504" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B504" s="3">
+        <v>9</v>
+      </c>
+      <c r="C504" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D504" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="505" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B505" s="3">
+        <v>10</v>
+      </c>
+      <c r="C505" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D505" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="506" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B506" s="3">
+        <v>11</v>
+      </c>
+      <c r="C506" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D506" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="507" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B507" s="3">
+        <v>12</v>
+      </c>
+      <c r="C507" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D507" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E507" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="508" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B508" s="3">
+        <v>13</v>
+      </c>
+      <c r="C508" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D508" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E508" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="509" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B509" s="3">
+        <v>14</v>
+      </c>
+      <c r="C509" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D509" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="510" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B510" s="3">
+        <v>15</v>
+      </c>
+      <c r="C510" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D510" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E510" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="511" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B511" s="3">
+        <v>16</v>
+      </c>
+      <c r="C511" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D511" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="512" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B512" s="3">
+        <v>17</v>
+      </c>
+      <c r="C512" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D512" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="513" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B513" s="3">
+        <v>18</v>
+      </c>
+      <c r="C513" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D513" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="514" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B514" s="3">
+        <v>19</v>
+      </c>
+      <c r="C514" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D514" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="515" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B515" s="3">
+        <v>20</v>
+      </c>
+      <c r="C515" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D515" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="516" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B516" s="3">
+        <v>21</v>
+      </c>
+      <c r="C516" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D516" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="517" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B517" s="3">
+        <v>22</v>
+      </c>
+      <c r="C517" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D517" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="518" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B518" s="3">
+        <v>23</v>
+      </c>
+      <c r="C518" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D518" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="519" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B519" s="3">
+        <v>24</v>
+      </c>
+      <c r="C519" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D519" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="520" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B520" s="3">
+        <v>25</v>
+      </c>
+      <c r="C520" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D520" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="521" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B521" s="3">
+        <v>26</v>
+      </c>
+      <c r="C521" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D521" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E521" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="522" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B522" s="3">
+        <v>27</v>
+      </c>
+      <c r="C522" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="D522" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="523" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B523" s="3">
+        <v>28</v>
+      </c>
+      <c r="C523" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D523" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="524" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B524" s="3">
+        <v>29</v>
+      </c>
+      <c r="C524" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D524" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="525" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B525" s="3">
+        <v>30</v>
+      </c>
+      <c r="C525" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D525" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="526" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B526" s="3">
+        <v>31</v>
+      </c>
+      <c r="C526" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D526" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="527" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B527" s="3">
+        <v>32</v>
+      </c>
+      <c r="C527" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D527" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="528" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B528" s="3">
+        <v>33</v>
+      </c>
+      <c r="C528" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D528" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="529" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B529" s="3">
+        <v>34</v>
+      </c>
+      <c r="C529" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="D529" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="530" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B530" s="3">
+        <v>35</v>
+      </c>
+      <c r="C530" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D530" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="531" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B531" s="3">
+        <v>36</v>
+      </c>
+      <c r="C531" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D531" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="532" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B532" s="3">
+        <v>37</v>
+      </c>
+      <c r="C532" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D532" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="533" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B533" s="3">
+        <v>38</v>
+      </c>
+      <c r="C533" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="D533" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="534" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B534" s="3">
+        <v>39</v>
+      </c>
+      <c r="C534" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D534" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="535" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B535" s="3">
+        <v>40</v>
+      </c>
+      <c r="C535" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D535" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="536" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B536" s="3">
+        <v>41</v>
+      </c>
+      <c r="C536" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="D536" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E536" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="537" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B537" s="3">
+        <v>42</v>
+      </c>
+      <c r="C537" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D537" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="538" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B538" s="3">
+        <v>43</v>
+      </c>
+      <c r="C538" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D538" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="539" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B539" s="3">
+        <v>44</v>
+      </c>
+      <c r="C539" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="D539" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="540" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B540" s="3">
+        <v>45</v>
+      </c>
+      <c r="C540" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D540" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E540" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="541" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B541" s="7">
+        <v>46</v>
+      </c>
+      <c r="C541" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="D541" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E541" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="542" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B542" s="3">
+        <v>47</v>
+      </c>
+      <c r="C542" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D542" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="543" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B543" s="3">
+        <v>48</v>
+      </c>
+      <c r="C543" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D543" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E543" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="544" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B544" s="3">
+        <v>49</v>
+      </c>
+      <c r="C544" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D544" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="545" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B545" s="3">
         <v>50</v>
       </c>
-      <c r="C503" s="3" t="s">
+      <c r="C545" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="D503" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E503" s="3" t="s">
+      <c r="D545" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E545" s="3" t="s">
         <v>321</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D380:K380"/>
-    <mergeCell ref="D386:K386"/>
+    <mergeCell ref="D422:K422"/>
+    <mergeCell ref="D428:K428"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F170" r:id="rId1"/>

</xml_diff>